<commit_message>
The updated task sheet with Data_Validation
</commit_message>
<xml_diff>
--- a/classs Tasks.xlsx
+++ b/classs Tasks.xlsx
@@ -2,21 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DA17\My GIT DATA\Task01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF545CB8-E865-4478-AB65-E7191B5EFD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A118FBC3-E369-486F-A9C2-85E9C117D87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{405E82EC-0242-4A65-8526-DF35E4A9BCA7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{405E82EC-0242-4A65-8526-DF35E4A9BCA7}"/>
   </bookViews>
   <sheets>
-    <sheet name="VLOOKUP" sheetId="1" r:id="rId1"/>
-    <sheet name="INDEX" sheetId="3" r:id="rId2"/>
-    <sheet name="MATCH" sheetId="4" r:id="rId3"/>
-    <sheet name="HLOOKUP" sheetId="2" r:id="rId4"/>
+    <sheet name="HLOOKUP" sheetId="2" r:id="rId1"/>
+    <sheet name="VLOOKUP" sheetId="1" r:id="rId2"/>
+    <sheet name="INDEX" sheetId="3" r:id="rId3"/>
+    <sheet name="MATCH" sheetId="4" r:id="rId4"/>
+    <sheet name="Data_Validation" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="30">
   <si>
     <t>Sujal</t>
   </si>
@@ -146,6 +147,9 @@
   </si>
   <si>
     <t>sana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DYNAMIC DATA VALIDATION </t>
   </si>
 </sst>
 </file>
@@ -169,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +222,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -246,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -258,6 +274,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,42 +296,42 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Marquee">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="5E5E5E"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="DDDDDD"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="418AB3"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="A6B727"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="F69200"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="838383"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="FEC306"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="DF5327"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="F59E00"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="B2B2B2"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -571,6 +589,488 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE22B127-0134-4239-A880-74C9EDC01D82}">
+  <dimension ref="D9:U22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>36</v>
+      </c>
+      <c r="F10" s="3">
+        <v>68</v>
+      </c>
+      <c r="G10" s="3">
+        <v>56</v>
+      </c>
+      <c r="H10" s="3">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3">
+        <v>24</v>
+      </c>
+      <c r="J10" s="3">
+        <v>58</v>
+      </c>
+      <c r="K10" s="3">
+        <f>SUM(E10:J10)</f>
+        <v>264</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="3">
+        <v>59</v>
+      </c>
+      <c r="P10" s="3">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>47</v>
+      </c>
+      <c r="R10" s="3">
+        <v>67</v>
+      </c>
+      <c r="S10" s="3">
+        <v>43</v>
+      </c>
+      <c r="T10" s="3">
+        <v>43</v>
+      </c>
+      <c r="U10" s="3">
+        <f>SUM(O10:T10)</f>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3">
+        <v>33</v>
+      </c>
+      <c r="H11" s="3">
+        <v>20</v>
+      </c>
+      <c r="I11" s="3">
+        <v>24</v>
+      </c>
+      <c r="J11" s="3">
+        <v>47</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" ref="K11:K22" si="0">SUM(E11:J11)</f>
+        <v>170</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="3">
+        <v>33</v>
+      </c>
+      <c r="P11" s="3">
+        <v>67</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>23</v>
+      </c>
+      <c r="R11" s="3">
+        <v>55</v>
+      </c>
+      <c r="S11" s="3">
+        <v>24</v>
+      </c>
+      <c r="T11" s="3">
+        <v>56</v>
+      </c>
+      <c r="U11" s="3">
+        <f>SUM(O11:T11)</f>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>33</v>
+      </c>
+      <c r="F12" s="3">
+        <v>32</v>
+      </c>
+      <c r="G12" s="3">
+        <v>27</v>
+      </c>
+      <c r="H12" s="3">
+        <v>40</v>
+      </c>
+      <c r="I12" s="3">
+        <v>34</v>
+      </c>
+      <c r="J12" s="3">
+        <v>58</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="0"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3">
+        <v>59</v>
+      </c>
+      <c r="F13" s="3">
+        <v>40</v>
+      </c>
+      <c r="G13" s="3">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3">
+        <v>65</v>
+      </c>
+      <c r="I13" s="3">
+        <v>57</v>
+      </c>
+      <c r="J13" s="3">
+        <v>32</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="0"/>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="3">
+        <v>41</v>
+      </c>
+      <c r="F14" s="3">
+        <v>39</v>
+      </c>
+      <c r="G14" s="3">
+        <v>47</v>
+      </c>
+      <c r="H14" s="3">
+        <v>21</v>
+      </c>
+      <c r="I14" s="3">
+        <v>33</v>
+      </c>
+      <c r="J14" s="3">
+        <v>24</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="0"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <f>HLOOKUP(E9,$N$9:$U$11,2,FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" ref="F15:K15" si="1">HLOOKUP(F9,$N$9:$U$11,2,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="1"/>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3">
+        <v>25</v>
+      </c>
+      <c r="G16" s="3">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3">
+        <v>61</v>
+      </c>
+      <c r="I16" s="3">
+        <v>45</v>
+      </c>
+      <c r="J16" s="3">
+        <v>46</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="0"/>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3">
+        <v>37</v>
+      </c>
+      <c r="F17" s="3">
+        <v>63</v>
+      </c>
+      <c r="G17" s="3">
+        <v>26</v>
+      </c>
+      <c r="H17" s="3">
+        <v>42</v>
+      </c>
+      <c r="I17" s="3">
+        <v>47</v>
+      </c>
+      <c r="J17" s="3">
+        <v>45</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3">
+        <v>58</v>
+      </c>
+      <c r="F18" s="3">
+        <v>21</v>
+      </c>
+      <c r="G18" s="3">
+        <v>66</v>
+      </c>
+      <c r="H18" s="3">
+        <v>24</v>
+      </c>
+      <c r="I18" s="3">
+        <v>48</v>
+      </c>
+      <c r="J18" s="3">
+        <v>49</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="0"/>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3">
+        <v>21</v>
+      </c>
+      <c r="F19" s="3">
+        <v>65</v>
+      </c>
+      <c r="G19" s="3">
+        <v>25</v>
+      </c>
+      <c r="H19" s="3">
+        <v>46</v>
+      </c>
+      <c r="I19" s="3">
+        <v>48</v>
+      </c>
+      <c r="J19" s="3">
+        <v>62</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="0"/>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="3">
+        <v>55</v>
+      </c>
+      <c r="F20" s="3">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3">
+        <v>35</v>
+      </c>
+      <c r="H20" s="3">
+        <v>62</v>
+      </c>
+      <c r="I20" s="3">
+        <v>21</v>
+      </c>
+      <c r="J20" s="3">
+        <v>22</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4">
+        <f>HLOOKUP(E9,$N$9:$U$11,3,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" ref="F21:K21" si="2">HLOOKUP(F9,$N$9:$U$11,3,FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="2"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="3">
+        <v>69</v>
+      </c>
+      <c r="F22" s="3">
+        <v>65</v>
+      </c>
+      <c r="G22" s="3">
+        <v>33</v>
+      </c>
+      <c r="H22" s="3">
+        <v>60</v>
+      </c>
+      <c r="I22" s="3">
+        <v>47</v>
+      </c>
+      <c r="J22" s="3">
+        <v>40</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="0"/>
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB6F745-7FFF-4165-BE5D-8E71ACE924E5}">
   <dimension ref="D6:P19"/>
   <sheetViews>
@@ -1106,7 +1606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12BA20B-BA0F-4F86-BB81-ABD8E270FE11}">
   <dimension ref="D9:O22"/>
   <sheetViews>
@@ -1517,11 +2017,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC6B50-5895-44F0-B26B-41B874F5B9DB}">
   <dimension ref="D7:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1939,484 +2439,314 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE22B127-0134-4239-A880-74C9EDC01D82}">
-  <dimension ref="D9:U22"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF24E35-C183-4312-8339-AEDCBB6630D7}">
+  <dimension ref="D8:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D9" s="1" t="s">
+    <row r="8" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="1" t="s">
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>17</v>
+      </c>
+      <c r="F13" s="12">
+        <v>17</v>
+      </c>
+      <c r="G13" s="12">
+        <v>12</v>
+      </c>
+      <c r="H13" s="12">
+        <v>7</v>
+      </c>
+      <c r="I13" s="12">
+        <v>9</v>
+      </c>
+      <c r="J13" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>9</v>
+      </c>
+      <c r="F14" s="12">
+        <v>16</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>4</v>
+      </c>
+      <c r="I14" s="12">
+        <v>15</v>
+      </c>
+      <c r="J14" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="12">
+        <v>10</v>
+      </c>
+      <c r="F15" s="12">
+        <v>16</v>
+      </c>
+      <c r="G15" s="12">
+        <v>2</v>
+      </c>
+      <c r="H15" s="12">
+        <v>3</v>
+      </c>
+      <c r="I15" s="12">
+        <v>8</v>
+      </c>
+      <c r="J15" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="12">
+        <v>12</v>
+      </c>
+      <c r="F16" s="12">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12">
+        <v>6</v>
+      </c>
+      <c r="H16" s="12">
+        <v>3</v>
+      </c>
+      <c r="I16" s="12">
+        <v>14</v>
+      </c>
+      <c r="J16" s="12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="12">
+        <v>3</v>
+      </c>
+      <c r="F17" s="12">
+        <v>12</v>
+      </c>
+      <c r="G17" s="12">
+        <v>11</v>
+      </c>
+      <c r="H17" s="12">
+        <v>19</v>
+      </c>
+      <c r="I17" s="12">
         <v>13</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P9" s="2" t="s">
+      <c r="J17" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="12">
+        <v>9</v>
+      </c>
+      <c r="F18" s="12">
+        <v>8</v>
+      </c>
+      <c r="G18" s="12">
+        <v>19</v>
+      </c>
+      <c r="H18" s="12">
+        <v>17</v>
+      </c>
+      <c r="I18" s="12">
+        <v>11</v>
+      </c>
+      <c r="J18" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="12">
+        <v>17</v>
+      </c>
+      <c r="F19" s="12">
+        <v>11</v>
+      </c>
+      <c r="G19" s="12">
+        <v>7</v>
+      </c>
+      <c r="H19" s="12">
+        <v>9</v>
+      </c>
+      <c r="I19" s="12">
+        <v>20</v>
+      </c>
+      <c r="J19" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="12">
+        <v>13</v>
+      </c>
+      <c r="F20" s="12">
+        <v>17</v>
+      </c>
+      <c r="G20" s="12">
+        <v>16</v>
+      </c>
+      <c r="H20" s="12">
+        <v>10</v>
+      </c>
+      <c r="I20" s="12">
+        <v>12</v>
+      </c>
+      <c r="J20" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="12">
+        <v>3</v>
+      </c>
+      <c r="F21" s="12">
+        <v>9</v>
+      </c>
+      <c r="G21" s="12">
+        <v>20</v>
+      </c>
+      <c r="H21" s="12">
+        <v>17</v>
+      </c>
+      <c r="I21" s="12">
+        <v>12</v>
+      </c>
+      <c r="J21" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="12">
+        <v>3</v>
+      </c>
+      <c r="F22" s="12">
+        <v>17</v>
+      </c>
+      <c r="G22" s="12">
+        <v>17</v>
+      </c>
+      <c r="H22" s="12">
+        <v>10</v>
+      </c>
+      <c r="I22" s="12">
+        <v>2</v>
+      </c>
+      <c r="J22" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="12">
+        <v>4</v>
+      </c>
+      <c r="F23" s="12">
+        <v>4</v>
+      </c>
+      <c r="G23" s="12">
+        <v>12</v>
+      </c>
+      <c r="H23" s="12">
+        <v>13</v>
+      </c>
+      <c r="I23" s="12">
         <v>15</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R9" s="2" t="s">
+      <c r="J23" s="12">
         <v>17</v>
       </c>
-      <c r="S9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>36</v>
-      </c>
-      <c r="F10" s="3">
-        <v>68</v>
-      </c>
-      <c r="G10" s="3">
-        <v>56</v>
-      </c>
-      <c r="H10" s="3">
-        <v>22</v>
-      </c>
-      <c r="I10" s="3">
-        <v>24</v>
-      </c>
-      <c r="J10" s="3">
-        <v>58</v>
-      </c>
-      <c r="K10" s="3">
-        <f>SUM(E10:J10)</f>
-        <v>264</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O10" s="3">
-        <v>59</v>
-      </c>
-      <c r="P10" s="3">
-        <v>33</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>47</v>
-      </c>
-      <c r="R10" s="3">
-        <v>67</v>
-      </c>
-      <c r="S10" s="3">
-        <v>43</v>
-      </c>
-      <c r="T10" s="3">
-        <v>43</v>
-      </c>
-      <c r="U10" s="3">
-        <f>SUM(O10:T10)</f>
-        <v>292</v>
-      </c>
-    </row>
-    <row r="11" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3">
-        <v>26</v>
-      </c>
-      <c r="F11" s="3">
-        <v>20</v>
-      </c>
-      <c r="G11" s="3">
-        <v>33</v>
-      </c>
-      <c r="H11" s="3">
-        <v>20</v>
-      </c>
-      <c r="I11" s="3">
-        <v>24</v>
-      </c>
-      <c r="J11" s="3">
-        <v>47</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" ref="K11:K22" si="0">SUM(E11:J11)</f>
-        <v>170</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="3">
-        <v>33</v>
-      </c>
-      <c r="P11" s="3">
-        <v>67</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>23</v>
-      </c>
-      <c r="R11" s="3">
-        <v>55</v>
-      </c>
-      <c r="S11" s="3">
-        <v>24</v>
-      </c>
-      <c r="T11" s="3">
-        <v>56</v>
-      </c>
-      <c r="U11" s="3">
-        <f>SUM(O11:T11)</f>
-        <v>258</v>
-      </c>
-    </row>
-    <row r="12" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3">
-        <v>33</v>
-      </c>
-      <c r="F12" s="3">
-        <v>32</v>
-      </c>
-      <c r="G12" s="3">
-        <v>27</v>
-      </c>
-      <c r="H12" s="3">
-        <v>40</v>
-      </c>
-      <c r="I12" s="3">
-        <v>34</v>
-      </c>
-      <c r="J12" s="3">
-        <v>58</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="0"/>
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3">
-        <v>59</v>
-      </c>
-      <c r="F13" s="3">
-        <v>40</v>
-      </c>
-      <c r="G13" s="3">
-        <v>21</v>
-      </c>
-      <c r="H13" s="3">
-        <v>65</v>
-      </c>
-      <c r="I13" s="3">
-        <v>57</v>
-      </c>
-      <c r="J13" s="3">
-        <v>32</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="0"/>
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="3">
-        <v>41</v>
-      </c>
-      <c r="F14" s="3">
-        <v>39</v>
-      </c>
-      <c r="G14" s="3">
-        <v>47</v>
-      </c>
-      <c r="H14" s="3">
-        <v>21</v>
-      </c>
-      <c r="I14" s="3">
-        <v>33</v>
-      </c>
-      <c r="J14" s="3">
-        <v>24</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="0"/>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4">
-        <f>HLOOKUP(E9,$N$9:$U$11,2,FALSE)</f>
-        <v>59</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" ref="F15:K15" si="1">HLOOKUP(F9,$N$9:$U$11,2,FALSE)</f>
-        <v>33</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="K15" s="4">
-        <f t="shared" si="1"/>
-        <v>292</v>
-      </c>
-    </row>
-    <row r="16" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="3">
-        <v>28</v>
-      </c>
-      <c r="F16" s="3">
-        <v>25</v>
-      </c>
-      <c r="G16" s="3">
-        <v>54</v>
-      </c>
-      <c r="H16" s="3">
-        <v>61</v>
-      </c>
-      <c r="I16" s="3">
-        <v>45</v>
-      </c>
-      <c r="J16" s="3">
-        <v>46</v>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" si="0"/>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3">
-        <v>37</v>
-      </c>
-      <c r="F17" s="3">
-        <v>63</v>
-      </c>
-      <c r="G17" s="3">
-        <v>26</v>
-      </c>
-      <c r="H17" s="3">
-        <v>42</v>
-      </c>
-      <c r="I17" s="3">
-        <v>47</v>
-      </c>
-      <c r="J17" s="3">
-        <v>45</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="0"/>
-        <v>260</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3">
-        <v>58</v>
-      </c>
-      <c r="F18" s="3">
-        <v>21</v>
-      </c>
-      <c r="G18" s="3">
-        <v>66</v>
-      </c>
-      <c r="H18" s="3">
-        <v>24</v>
-      </c>
-      <c r="I18" s="3">
-        <v>48</v>
-      </c>
-      <c r="J18" s="3">
-        <v>49</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="0"/>
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="3">
-        <v>21</v>
-      </c>
-      <c r="F19" s="3">
-        <v>65</v>
-      </c>
-      <c r="G19" s="3">
-        <v>25</v>
-      </c>
-      <c r="H19" s="3">
-        <v>46</v>
-      </c>
-      <c r="I19" s="3">
-        <v>48</v>
-      </c>
-      <c r="J19" s="3">
-        <v>62</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="0"/>
-        <v>267</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="3">
-        <v>55</v>
-      </c>
-      <c r="F20" s="3">
-        <v>61</v>
-      </c>
-      <c r="G20" s="3">
-        <v>35</v>
-      </c>
-      <c r="H20" s="3">
-        <v>62</v>
-      </c>
-      <c r="I20" s="3">
-        <v>21</v>
-      </c>
-      <c r="J20" s="3">
-        <v>22</v>
-      </c>
-      <c r="K20" s="3">
-        <f t="shared" si="0"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="4">
-        <f>HLOOKUP(E9,$N$9:$U$11,3,FALSE)</f>
-        <v>33</v>
-      </c>
-      <c r="F21" s="4">
-        <f t="shared" ref="F21:K21" si="2">HLOOKUP(F9,$N$9:$U$11,3,FALSE)</f>
-        <v>67</v>
-      </c>
-      <c r="G21" s="4">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-      <c r="K21" s="4">
-        <f t="shared" si="2"/>
-        <v>258</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="3">
-        <v>69</v>
-      </c>
-      <c r="F22" s="3">
-        <v>65</v>
-      </c>
-      <c r="G22" s="3">
-        <v>33</v>
-      </c>
-      <c r="H22" s="3">
-        <v>60</v>
-      </c>
-      <c r="I22" s="3">
-        <v>47</v>
-      </c>
-      <c r="J22" s="3">
-        <v>40</v>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" si="0"/>
-        <v>314</v>
-      </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:J23" xr:uid="{91D6D0C4-8838-4BE0-950A-6607ABF38CC6}">
+      <formula1>1</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning only!!!" error="Read input message carefully and after that enter the numbers" promptTitle="Whole number only" prompt="Enter numbers should satisfie the condition and that is between 1 to 20" sqref="E13:J23" xr:uid="{104B49C8-629B-408F-841C-3AD05E2024BA}">
+      <formula1>1</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>